<commit_message>
update existing employee job
</commit_message>
<xml_diff>
--- a/src/test/java/com/pack/testData/StatusEmployee.xlsx
+++ b/src/test/java/com/pack/testData/StatusEmployee.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
     <t>EmpId</t>
   </si>
@@ -137,6 +137,90 @@
   </si>
   <si>
     <t>Tom</t>
+  </si>
+  <si>
+    <t>111111</t>
+  </si>
+  <si>
+    <t>002695</t>
+  </si>
+  <si>
+    <t>000504</t>
+  </si>
+  <si>
+    <t>002031</t>
+  </si>
+  <si>
+    <t>222294</t>
+  </si>
+  <si>
+    <t>123 Main St</t>
+  </si>
+  <si>
+    <t>234 Main St</t>
+  </si>
+  <si>
+    <t xml:space="preserve">234 Durham </t>
+  </si>
+  <si>
+    <t>ln</t>
+  </si>
+  <si>
+    <t>234 Durham Ln</t>
+  </si>
+  <si>
+    <t>325 MLK BLVD</t>
+  </si>
+  <si>
+    <t>455 Dearborn Ave</t>
+  </si>
+  <si>
+    <t>3114 Rudder Ln</t>
+  </si>
+  <si>
+    <t>987 Express Parkway</t>
+  </si>
+  <si>
+    <t>5443 Glenbridge Rd</t>
+  </si>
+  <si>
+    <t>San Antonio</t>
+  </si>
+  <si>
+    <t>5678 Hemingway St</t>
+  </si>
+  <si>
+    <t>67677 Lyyod St</t>
+  </si>
+  <si>
+    <t>67677 Lord St</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>234563</t>
+  </si>
+  <si>
+    <t>002542</t>
+  </si>
+  <si>
+    <t>000727</t>
+  </si>
+  <si>
+    <t>000065</t>
+  </si>
+  <si>
+    <t>002595</t>
+  </si>
+  <si>
+    <t>002756</t>
+  </si>
+  <si>
+    <t>000002</t>
+  </si>
+  <si>
+    <t>002452</t>
   </si>
 </sst>
 </file>
@@ -493,10 +577,10 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A11" sqref="A11" activeCellId="0"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
@@ -505,7 +589,7 @@
     <col min="7" max="7" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -528,21 +612,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
+        <v>42</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>56</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
       </c>
       <c r="E2">
-        <v>501510</v>
+        <v>60176</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -551,21 +635,21 @@
         <v>44542</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
+        <v>43</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>56</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
       </c>
       <c r="E3">
-        <v>501511</v>
+        <v>60608</v>
       </c>
       <c r="F3" t="s">
         <v>13</v>
@@ -574,21 +658,21 @@
         <v>44542</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
+        <v>46</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>56</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
       </c>
       <c r="E4">
-        <v>501512</v>
+        <v>60612</v>
       </c>
       <c r="F4" t="s">
         <v>16</v>
@@ -597,21 +681,21 @@
         <v>44542</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
+        <v>47</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>56</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
       </c>
       <c r="E5">
-        <v>501513</v>
+        <v>60609</v>
       </c>
       <c r="F5" t="s">
         <v>19</v>
@@ -620,21 +704,21 @@
         <v>44542</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
+        <v>48</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>56</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
       </c>
       <c r="E6">
-        <v>501514</v>
+        <v>60618</v>
       </c>
       <c r="F6" t="s">
         <v>22</v>
@@ -643,21 +727,21 @@
         <v>44542</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
+        <v>49</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>56</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
       </c>
       <c r="E7">
-        <v>501515</v>
+        <v>60610</v>
       </c>
       <c r="F7" t="s">
         <v>25</v>
@@ -666,21 +750,21 @@
         <v>44542</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
+        <v>50</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>56</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
       </c>
       <c r="E8">
-        <v>501516</v>
+        <v>60614</v>
       </c>
       <c r="F8" t="s">
         <v>27</v>
@@ -689,21 +773,21 @@
         <v>44542</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" t="s">
-        <v>29</v>
+        <v>51</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>56</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
       </c>
       <c r="E9">
-        <v>501517</v>
+        <v>60617</v>
       </c>
       <c r="F9" t="s">
         <v>30</v>
@@ -712,21 +796,21 @@
         <v>44542</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" t="s">
-        <v>32</v>
+        <v>53</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>56</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
       </c>
       <c r="E10">
-        <v>501518</v>
+        <v>60618</v>
       </c>
       <c r="F10" t="s">
         <v>33</v>
@@ -735,21 +819,21 @@
         <v>44542</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" t="s">
-        <v>35</v>
+        <v>55</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>56</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
       </c>
       <c r="E11">
-        <v>501519</v>
+        <v>60611</v>
       </c>
       <c r="F11" t="s">
         <v>36</v>

</xml_diff>